<commit_message>
Week 5 Assignment Complete
</commit_message>
<xml_diff>
--- a/Homework/Assignment_4/israeli_vaccination_data_analysis_start.xlsx
+++ b/Homework/Assignment_4/israeli_vaccination_data_analysis_start.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="84" documentId="8_{5549D065-8479-439F-98C9-6763E114659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5880A9C-884B-45E6-9471-F5E93C6915BE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3BC2D1D-D8A4-4834-AFE1-B059B15AE70E}"/>
+    <workbookView xWindow="5490" yWindow="4455" windowWidth="17280" windowHeight="9150" xr2:uid="{F3BC2D1D-D8A4-4834-AFE1-B059B15AE70E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>